<commit_message>
Restructure code to read the product and item from excel sheet and update record in products table.
</commit_message>
<xml_diff>
--- a/dhs/dhs/scripts/Products.xlsx
+++ b/dhs/dhs/scripts/Products.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svivek\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svivek\Downloads\dhs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -162,10 +162,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,7 +474,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,16 +516,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
@@ -539,14 +539,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
@@ -560,16 +560,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
@@ -583,14 +583,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
@@ -604,14 +604,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
@@ -625,14 +625,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
@@ -646,16 +646,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
@@ -669,14 +669,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
@@ -690,14 +690,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E10" t="s">
@@ -711,14 +711,14 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
@@ -732,16 +732,16 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
@@ -755,14 +755,14 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
@@ -776,14 +776,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
@@ -797,14 +797,14 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" t="s">

</xml_diff>

<commit_message>
Unit Support is added.
</commit_message>
<xml_diff>
--- a/dhs/dhs/scripts/Products.xlsx
+++ b/dhs/dhs/scripts/Products.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>Kabja Lory</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Initial Stock</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Minimum Threshhold</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
     <t>100 Bori</t>
   </si>
   <si>
-    <t>Weighing Units</t>
-  </si>
-  <si>
-    <t>Kg, Bori</t>
-  </si>
-  <si>
     <t>Kabja ISI VIP 3 Inch</t>
   </si>
   <si>
@@ -117,13 +108,46 @@
     <t>50 Bori</t>
   </si>
   <si>
-    <t>900 Kg</t>
-  </si>
-  <si>
     <t>Kabja ISI SRI RAM</t>
   </si>
   <si>
     <t>Item Code</t>
+  </si>
+  <si>
+    <t>Hex Bolt</t>
+  </si>
+  <si>
+    <t>HB Full Thread 2 sut 1 inch</t>
+  </si>
+  <si>
+    <t>25 Kg = 1 Bori</t>
+  </si>
+  <si>
+    <t>10 Bori</t>
+  </si>
+  <si>
+    <t>20 Bori</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>kg = 70, Bori = 1700</t>
+  </si>
+  <si>
+    <t>kg = 50, Bori = 1000</t>
+  </si>
+  <si>
+    <t>kg = 50, Bori = 1500</t>
+  </si>
+  <si>
+    <t>kg = 100, Bori = 2500</t>
+  </si>
+  <si>
+    <t>kg = 200, Bori = 6000</t>
+  </si>
+  <si>
+    <t>300 Bori</t>
   </si>
 </sst>
 </file>
@@ -471,39 +495,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -511,11 +534,8 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,20 +545,17 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>2</v>
@@ -546,275 +563,256 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
-        <v>1000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>600</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>600</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>600</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>600</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>800</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>800</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>800</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>800</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12">
-        <v>800</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13">
-        <v>800</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14">
-        <v>800</v>
-      </c>
-      <c r="G14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="F15">
-        <v>800</v>
-      </c>
-      <c r="G15" t="s">
-        <v>7</v>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes: 1. Added basic code to print the sale order on printer. 2. Minor style changes.
</commit_message>
<xml_diff>
--- a/dhs/dhs/scripts/Products.xlsx
+++ b/dhs/dhs/scripts/Products.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
   <si>
     <t>Kabja Lory</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>300 Bori</t>
+  </si>
+  <si>
+    <t>HB Full Thread 2 sut 2 inch</t>
+  </si>
+  <si>
+    <t>HB Full Thread 2 sut 3 inch</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,7 +802,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
@@ -815,12 +821,49 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>